<commit_message>
Set up test folders and copyFiles
</commit_message>
<xml_diff>
--- a/Test/2016.116 - A test project folder/Project_Information.xlsx
+++ b/Test/2016.116 - A test project folder/Project_Information.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="7520" windowWidth="28160" windowHeight="21020" tabRatio="500"/>
+    <workbookView xWindow="22480" yWindow="300" windowWidth="28160" windowHeight="21020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Project Database Builder</t>
   </si>
@@ -30,6 +30,9 @@
     <t>Type</t>
   </si>
   <si>
+    <t>Revit or CAD</t>
+  </si>
+  <si>
     <t>e.g.: 415 N. Mathilda Market Ready</t>
   </si>
   <si>
@@ -91,24 +94,6 @@
   </si>
   <si>
     <t>299 Bassett St. #250</t>
-  </si>
-  <si>
-    <t>Project Number</t>
-  </si>
-  <si>
-    <t>Project Manager</t>
-  </si>
-  <si>
-    <t>Tim</t>
-  </si>
-  <si>
-    <t>Person in charge</t>
-  </si>
-  <si>
-    <t>e.g. 2016.21</t>
-  </si>
-  <si>
-    <t>Revit or CAD or Other</t>
   </si>
 </sst>
 </file>
@@ -197,31 +182,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="6">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -554,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -574,129 +552,107 @@
     </row>
     <row r="2" spans="1:3">
       <c r="B2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="5">
-        <v>2016.116</v>
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="2" t="s">
+    <row r="16" spans="1:3">
+      <c r="B16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="B13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="B14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="B15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="B18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B15" r:id="rId1"/>
+    <hyperlink ref="B13" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>